<commit_message>
Folder Refractor and Python Program Debugging
</commit_message>
<xml_diff>
--- a/dump/test.xlsx
+++ b/dump/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64931733c3934785/Documents/Q4 2022/Fishing Tournament 2021 Repos/dump/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64931733c3934785/Documents/Q4 2022/Proyecto de Graduacion Fase I/Fishing Tournament 2021 Repos/gui/dump/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_46DD91AB5F82495A5AB01DFFAC26882B4E6F449B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78C6B63B-526A-4AB5-99F4-CCA22A6F27B9}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_47CD50A45F82495A5AB01DB3D407A32473416231" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56FD1F6B-02D2-4913-8CD0-C3C740330269}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="3360" windowWidth="14970" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,24 @@
     <sheet name="Kids" sheetId="5" r:id="rId5"/>
     <sheet name="Women" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -57,26 +69,55 @@
     <t>WOMEN_PRESENT</t>
   </si>
   <si>
-    <t>Bote</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(123) 456-7890
-</t>
-  </si>
-  <si>
-    <t>marzo651@gmail.com</t>
+    <t>PARTICIPATION FEE</t>
+  </si>
+  <si>
+    <t>TOTAL FEES</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>Robin Arellano</t>
+  </si>
+  <si>
+    <t>(102)555 5555</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
   </si>
   <si>
     <t>Participating</t>
+  </si>
+  <si>
+    <t>Olimpic</t>
+  </si>
+  <si>
+    <t>Bobby Schwalter</t>
+  </si>
+  <si>
+    <t>Costic</t>
+  </si>
+  <si>
+    <t>Genghis Khan</t>
+  </si>
+  <si>
+    <t>Costa Concordia</t>
+  </si>
+  <si>
+    <t>Reventuki Reventar</t>
+  </si>
+  <si>
+    <t>Not Participating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,27 +452,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,37 +505,159 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <f>IF(F2="Participating",700,0)+IF(G2="Participating",350,0)+IF(H2="Participating",300,0)+IF(I2="Participating",50,0)+IF(J2="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+      <c r="N2" s="1">
+        <f>SUM(K:K)</f>
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <f>IF(F3="Participating",700,0)+IF(G3="Participating",350,0)+IF(H3="Participating",300,0)+IF(I3="Participating",50,0)+IF(J3="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f>IF(F4="Participating",700,0)+IF(G4="Participating",350,0)+IF(H4="Participating",300,0)+IF(I4="Participating",50,0)+IF(J4="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <f>VALUE(IF(F5="Participating",700,0)+IF(G5="Participating",350,0)+IF(H5="Participating",300,0)+IF(I5="Participating",50,0)+IF(J5="Participating",50,0))</f>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -515,9 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -529,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>